<commit_message>
updated readme and project tracking
</commit_message>
<xml_diff>
--- a/Resources/Project Summary.xlsx
+++ b/Resources/Project Summary.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\msu\20 - Final Project\group_project\References\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\msu\20 - Final Project\group_project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAD130D-60F1-47DC-9259-4209ECC5BB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A6CD46-6329-4633-A8E4-023B4B862CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="0" windowWidth="25845" windowHeight="15600" activeTab="4" xr2:uid="{241C9D2D-BDEA-4EB4-AA6E-D41C381F1952}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{241C9D2D-BDEA-4EB4-AA6E-D41C381F1952}"/>
   </bookViews>
   <sheets>
-    <sheet name="Physician Data" sheetId="11" r:id="rId1"/>
+    <sheet name="1st Segment" sheetId="14" r:id="rId1"/>
     <sheet name="Summary" sheetId="8" r:id="rId2"/>
-    <sheet name="References" sheetId="9" r:id="rId3"/>
-    <sheet name="Grade" sheetId="2" r:id="rId4"/>
+    <sheet name="Physician Data" sheetId="11" r:id="rId3"/>
+    <sheet name="References" sheetId="9" r:id="rId4"/>
     <sheet name="Notes" sheetId="12" r:id="rId5"/>
     <sheet name="Limitations" sheetId="13" r:id="rId6"/>
+    <sheet name="Grade" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Physician Data'!$A$1:$E$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Physician Data'!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="176">
   <si>
     <t>Project</t>
   </si>
@@ -507,6 +508,74 @@
   </si>
   <si>
     <t>Resolve issue with pushing to github</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Selected topic </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reason why they selected their topic </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description of their source of data </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Takes in data in from the provisional database </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sample data that mimics the expected final database structure or schema </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Questions they hope to answer with the data</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Machine Learning Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Includes a README.md README.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> README.md must include: Description of the communication protocols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual Branches: At least one branch for each team member </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Each team member has at least four commits from the duration of the first segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outputs label(s) for input data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Draft machine learning module is connected to the provisional database</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Points
+Avail</t>
+  </si>
+  <si>
+    <t>Points
+Scored</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
@@ -568,7 +637,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -943,12 +1012,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1065,31 +1182,70 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1414,6 +1570,1121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE6C3A-695D-44EF-B92F-86DBEA14E3DC}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="57">
+        <v>30</v>
+      </c>
+      <c r="E2" s="59"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="49"/>
+      <c r="B3" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="53"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
+      <c r="B4" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="53"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50"/>
+      <c r="B5" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="54"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="58"/>
+      <c r="D6" s="57">
+        <v>10</v>
+      </c>
+      <c r="E6" s="59"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="53"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="53"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50"/>
+      <c r="B9" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="52"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="54"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="57">
+        <v>35</v>
+      </c>
+      <c r="E10" s="59"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50"/>
+      <c r="B11" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="52"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="54"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="58"/>
+      <c r="D12" s="57">
+        <v>25</v>
+      </c>
+      <c r="E12" s="59"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50"/>
+      <c r="B13" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="52"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="54"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60">
+        <f>SUM(D2:D13)</f>
+        <v>100</v>
+      </c>
+      <c r="E14" s="60">
+        <f>SUM(E2:E13)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C852F2-FAA5-4B27-AD13-24C7EB26B87C}">
+  <dimension ref="A1:G72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="23">
+        <v>44594</v>
+      </c>
+      <c r="G3" s="16">
+        <v>44587</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
+      <c r="B4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="17">
+        <v>44594</v>
+      </c>
+      <c r="G4" s="18">
+        <v>44587</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="41"/>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="17">
+        <v>44594</v>
+      </c>
+      <c r="G6" s="18">
+        <v>44587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="B10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="46"/>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46"/>
+      <c r="B16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="41"/>
+      <c r="B20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="46"/>
+      <c r="B21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="44"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="41"/>
+      <c r="B26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="41"/>
+      <c r="B28" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="41"/>
+      <c r="B29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="41"/>
+      <c r="B30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="41"/>
+      <c r="B33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="48"/>
+      <c r="B34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="46"/>
+      <c r="B35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="46"/>
+      <c r="B38" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="44"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="41"/>
+      <c r="B43" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+    </row>
+    <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="41"/>
+      <c r="B44" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+    </row>
+    <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="41"/>
+      <c r="B45" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="41"/>
+      <c r="B46" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="41"/>
+      <c r="B47" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+    </row>
+    <row r="48" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="41"/>
+      <c r="B48" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="41"/>
+      <c r="B49" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="41"/>
+      <c r="B50" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="41"/>
+      <c r="B51" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+    </row>
+    <row r="52" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="41"/>
+      <c r="B52" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="46"/>
+      <c r="B53" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="12"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="43"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="44"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="41"/>
+      <c r="B58" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+    </row>
+    <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="41"/>
+      <c r="B59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+    </row>
+    <row r="60" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="41"/>
+      <c r="B60" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+    </row>
+    <row r="61" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="41"/>
+      <c r="B61" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+    </row>
+    <row r="62" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="41"/>
+      <c r="B62" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="41"/>
+      <c r="B63" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+    </row>
+    <row r="64" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="41"/>
+      <c r="B64" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+    </row>
+    <row r="65" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="46"/>
+      <c r="B65" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="12"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="44"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="41"/>
+      <c r="B70" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="41"/>
+      <c r="B71" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="46"/>
+      <c r="B72" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A42:A53"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A23:G23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E729EE-DEDD-44FB-892C-76E3520BDE5B}">
   <dimension ref="A1:I41"/>
   <sheetViews>
@@ -2124,929 +3395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C852F2-FAA5-4B27-AD13-24C7EB26B87C}">
-  <dimension ref="A1:G72"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="23">
-        <v>44594</v>
-      </c>
-      <c r="G3" s="16">
-        <v>44587</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="17">
-        <v>44594</v>
-      </c>
-      <c r="G4" s="18">
-        <v>44587</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="17">
-        <v>44594</v>
-      </c>
-      <c r="G6" s="18">
-        <v>44587</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45"/>
-      <c r="B12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45"/>
-      <c r="B16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
-      <c r="B21" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-    </row>
-    <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
-      <c r="B34" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
-      <c r="B35" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" ht="2.4500000000000002" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
-      <c r="B38" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="42"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-      <c r="B43" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-    </row>
-    <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-    </row>
-    <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-    </row>
-    <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-    </row>
-    <row r="47" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="44"/>
-      <c r="B47" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-    </row>
-    <row r="48" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-    </row>
-    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-    </row>
-    <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-    </row>
-    <row r="52" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
-      <c r="B52" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="45"/>
-      <c r="B53" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-    </row>
-    <row r="54" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="42"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="G56" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-    </row>
-    <row r="58" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
-      <c r="B58" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-    </row>
-    <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
-      <c r="B59" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-    </row>
-    <row r="60" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="44"/>
-      <c r="B60" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-    </row>
-    <row r="61" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
-      <c r="B61" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-    </row>
-    <row r="62" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
-      <c r="B62" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9"/>
-    </row>
-    <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-    </row>
-    <row r="64" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="45"/>
-      <c r="B65" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-    </row>
-    <row r="66" spans="1:7" ht="2.4500000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="41"/>
-      <c r="G67" s="42"/>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C68" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D68" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E68" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F68" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-    </row>
-    <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="44"/>
-      <c r="B70" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="44"/>
-      <c r="B71" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
-    </row>
-    <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="45"/>
-      <c r="B72" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A42:A53"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A57:A65"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06689E2-AD35-403A-B277-1F7A6902B34D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3070,7 +3419,9 @@
       <c r="A2" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="26" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3088,99 +3439,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6778B80B-57A3-49F9-829D-BD3A1A351548}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7">
-        <f>C2*$B$2+C3*$B$3+C4*$B$4+C5*$B$5+C6*$B$6</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A43088F-BCEF-49C1-995E-3284D137F656}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3228,7 +3491,9 @@
       <c r="C3" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
@@ -3240,7 +3505,9 @@
       <c r="C4" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
@@ -3492,9 +3759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEDF1D8-3AEE-4455-9A00-39D4871E0119}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3761,4 +4026,91 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6778B80B-57A3-49F9-829D-BD3A1A351548}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="C2" s="6">
+        <f>'1st Segment'!E14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7">
+        <f>C2*$B$2+C3*$B$3+C4*$B$4+C5*$B$5+C6*$B$6</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formatted readme and updated prject tracking
</commit_message>
<xml_diff>
--- a/Resources/Project Summary.xlsx
+++ b/Resources/Project Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\msu\20 - Final Project\group_project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A6CD46-6329-4633-A8E4-023B4B862CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0847A0-8B78-4A59-9A0E-C3BBFBC46835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{241C9D2D-BDEA-4EB4-AA6E-D41C381F1952}"/>
+    <workbookView xWindow="-12390" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="4" xr2:uid="{241C9D2D-BDEA-4EB4-AA6E-D41C381F1952}"/>
   </bookViews>
   <sheets>
     <sheet name="1st Segment" sheetId="14" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Grade" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Notes!$A$1:$D$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Physician Data'!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="185">
   <si>
     <t>Project</t>
   </si>
@@ -495,9 +496,6 @@
     <t>Rearrange columns in merged data so that zip is first</t>
   </si>
   <si>
-    <t>Use different data source (Census) for income vs zip?</t>
-  </si>
-  <si>
     <t>Additional Info</t>
   </si>
   <si>
@@ -576,6 +574,36 @@
   </si>
   <si>
     <t>---</t>
+  </si>
+  <si>
+    <t>Use different data source (Census?) for income vs zip?</t>
+  </si>
+  <si>
+    <t>Use different data source for physicians?</t>
+  </si>
+  <si>
+    <t>Issue with having our physician data on github?</t>
+  </si>
+  <si>
+    <t>Logged by</t>
+  </si>
+  <si>
+    <t>Add third github branch for Jacqueline</t>
+  </si>
+  <si>
+    <t>Add other classification models?</t>
+  </si>
+  <si>
+    <t>Use Amazon S3 bucket?</t>
+  </si>
+  <si>
+    <t>Need to define output / add additional info (death rates?)</t>
+  </si>
+  <si>
+    <t>Use CenPy to connect to the census data?</t>
+  </si>
+  <si>
+    <t>How are we handling merges and branches?</t>
   </si>
 </sst>
 </file>
@@ -1182,70 +1210,70 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1573,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE6C3A-695D-44EF-B92F-86DBEA14E3DC}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1586,164 +1614,168 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="E1" s="56" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="47">
+        <v>30</v>
+      </c>
+      <c r="E2" s="50"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="48"/>
+      <c r="B3" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="51"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="51"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="49"/>
+      <c r="B5" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="52"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="47">
+        <v>10</v>
+      </c>
+      <c r="E6" s="50"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="48"/>
+      <c r="B7" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="51"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="51"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="49"/>
+      <c r="B9" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="52"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="47">
+        <v>35</v>
+      </c>
+      <c r="E10" s="50"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="B11" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="52"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="44"/>
+      <c r="D12" s="47">
+        <v>25</v>
+      </c>
+      <c r="E12" s="50"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="52"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="45" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="57">
-        <v>30</v>
-      </c>
-      <c r="E2" s="59"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="53"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="53"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
-      <c r="B5" s="52" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="54"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="57">
-        <v>10</v>
-      </c>
-      <c r="E6" s="59"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="53"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="53"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
-      <c r="B9" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="54"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
-        <v>163</v>
-      </c>
-      <c r="B10" s="58" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="57">
-        <v>35</v>
-      </c>
-      <c r="E10" s="59"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="54"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="58" t="s">
-        <v>159</v>
-      </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="57">
-        <v>25</v>
-      </c>
-      <c r="E12" s="59"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="54"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="60" t="s">
+      <c r="B14" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="B14" s="61" t="s">
-        <v>175</v>
-      </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60">
+      <c r="C14" s="45"/>
+      <c r="D14" s="45">
         <f>SUM(D2:D13)</f>
         <v>100</v>
       </c>
-      <c r="E14" s="60">
+      <c r="E14" s="45">
         <f>SUM(E2:E13)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A11"/>
@@ -1752,10 +1784,6 @@
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1779,15 +1807,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -1813,7 +1841,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="61" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -1836,7 +1864,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -1857,7 +1885,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1868,7 +1896,7 @@
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1889,7 +1917,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
@@ -1900,7 +1928,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
@@ -1911,7 +1939,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
@@ -1922,7 +1950,7 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
@@ -1933,7 +1961,7 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
@@ -1944,7 +1972,7 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="10" t="s">
         <v>19</v>
       </c>
@@ -1964,7 +1992,7 @@
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="56" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1977,7 +2005,7 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
@@ -1988,7 +2016,7 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="10" t="s">
         <v>23</v>
       </c>
@@ -2008,7 +2036,7 @@
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="60" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -2021,7 +2049,7 @@
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
@@ -2032,7 +2060,7 @@
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
@@ -2043,7 +2071,7 @@
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="46"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="10" t="s">
         <v>28</v>
       </c>
@@ -2063,15 +2091,15 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="44"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="55"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -2097,7 +2125,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="60" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -2110,7 +2138,7 @@
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="9" t="s">
         <v>39</v>
       </c>
@@ -2121,7 +2149,7 @@
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="9" t="s">
         <v>40</v>
       </c>
@@ -2132,7 +2160,7 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="9" t="s">
         <v>41</v>
       </c>
@@ -2143,7 +2171,7 @@
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="9" t="s">
         <v>42</v>
       </c>
@@ -2154,7 +2182,7 @@
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="9" t="s">
         <v>43</v>
       </c>
@@ -2174,7 +2202,7 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="56" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -2187,7 +2215,7 @@
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="57"/>
       <c r="B33" s="9" t="s">
         <v>45</v>
       </c>
@@ -2198,7 +2226,7 @@
       <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="9" t="s">
         <v>46</v>
       </c>
@@ -2209,7 +2237,7 @@
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
+      <c r="A35" s="58"/>
       <c r="B35" s="10" t="s">
         <v>47</v>
       </c>
@@ -2229,7 +2257,7 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="60" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -2242,7 +2270,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
+      <c r="A38" s="58"/>
       <c r="B38" s="10" t="s">
         <v>49</v>
       </c>
@@ -2262,15 +2290,15 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="55"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
@@ -2296,7 +2324,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="56" t="s">
         <v>51</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -2309,7 +2337,7 @@
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="9" t="s">
         <v>53</v>
       </c>
@@ -2320,7 +2348,7 @@
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
+      <c r="A44" s="57"/>
       <c r="B44" s="9" t="s">
         <v>54</v>
       </c>
@@ -2331,7 +2359,7 @@
       <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="9" t="s">
         <v>55</v>
       </c>
@@ -2342,7 +2370,7 @@
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="41"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="9" t="s">
         <v>56</v>
       </c>
@@ -2353,7 +2381,7 @@
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="41"/>
+      <c r="A47" s="57"/>
       <c r="B47" s="9" t="s">
         <v>57</v>
       </c>
@@ -2364,7 +2392,7 @@
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="41"/>
+      <c r="A48" s="57"/>
       <c r="B48" s="9" t="s">
         <v>58</v>
       </c>
@@ -2375,7 +2403,7 @@
       <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
+      <c r="A49" s="57"/>
       <c r="B49" s="9" t="s">
         <v>62</v>
       </c>
@@ -2386,7 +2414,7 @@
       <c r="G49" s="9"/>
     </row>
     <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="41"/>
+      <c r="A50" s="57"/>
       <c r="B50" s="9" t="s">
         <v>63</v>
       </c>
@@ -2397,7 +2425,7 @@
       <c r="G50" s="9"/>
     </row>
     <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="41"/>
+      <c r="A51" s="57"/>
       <c r="B51" s="9" t="s">
         <v>61</v>
       </c>
@@ -2408,7 +2436,7 @@
       <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="41"/>
+      <c r="A52" s="57"/>
       <c r="B52" s="9" t="s">
         <v>60</v>
       </c>
@@ -2419,7 +2447,7 @@
       <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="46"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="10" t="s">
         <v>59</v>
       </c>
@@ -2439,15 +2467,15 @@
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="42" t="s">
+      <c r="A55" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="44"/>
+      <c r="B55" s="54"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="55"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
@@ -2473,7 +2501,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="56" t="s">
         <v>51</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -2486,7 +2514,7 @@
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="41"/>
+      <c r="A58" s="57"/>
       <c r="B58" s="9" t="s">
         <v>71</v>
       </c>
@@ -2497,7 +2525,7 @@
       <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="41"/>
+      <c r="A59" s="57"/>
       <c r="B59" s="9" t="s">
         <v>72</v>
       </c>
@@ -2508,7 +2536,7 @@
       <c r="G59" s="9"/>
     </row>
     <row r="60" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="41"/>
+      <c r="A60" s="57"/>
       <c r="B60" s="9" t="s">
         <v>65</v>
       </c>
@@ -2519,7 +2547,7 @@
       <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
+      <c r="A61" s="57"/>
       <c r="B61" s="9" t="s">
         <v>66</v>
       </c>
@@ -2530,7 +2558,7 @@
       <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="41"/>
+      <c r="A62" s="57"/>
       <c r="B62" s="9" t="s">
         <v>67</v>
       </c>
@@ -2541,7 +2569,7 @@
       <c r="G62" s="9"/>
     </row>
     <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="41"/>
+      <c r="A63" s="57"/>
       <c r="B63" s="9" t="s">
         <v>68</v>
       </c>
@@ -2552,7 +2580,7 @@
       <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="41"/>
+      <c r="A64" s="57"/>
       <c r="B64" s="9" t="s">
         <v>69</v>
       </c>
@@ -2563,7 +2591,7 @@
       <c r="G64" s="9"/>
     </row>
     <row r="65" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="46"/>
+      <c r="A65" s="58"/>
       <c r="B65" s="10" t="s">
         <v>73</v>
       </c>
@@ -2583,15 +2611,15 @@
       <c r="G66" s="11"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="42" t="s">
+      <c r="A67" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="44"/>
+      <c r="B67" s="54"/>
+      <c r="C67" s="54"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="54"/>
+      <c r="F67" s="54"/>
+      <c r="G67" s="55"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
@@ -2617,7 +2645,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="47" t="s">
+      <c r="A69" s="56" t="s">
         <v>51</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -2630,7 +2658,7 @@
       <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="41"/>
+      <c r="A70" s="57"/>
       <c r="B70" s="9" t="s">
         <v>76</v>
       </c>
@@ -2641,7 +2669,7 @@
       <c r="G70" s="9"/>
     </row>
     <row r="71" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="41"/>
+      <c r="A71" s="57"/>
       <c r="B71" s="9" t="s">
         <v>77</v>
       </c>
@@ -2652,7 +2680,7 @@
       <c r="G71" s="9"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="46"/>
+      <c r="A72" s="58"/>
       <c r="B72" s="10" t="s">
         <v>78</v>
       </c>
@@ -2664,6 +2692,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A23:G23"/>
     <mergeCell ref="A67:G67"/>
     <mergeCell ref="A69:A72"/>
     <mergeCell ref="A32:A35"/>
@@ -2672,12 +2706,6 @@
     <mergeCell ref="A42:A53"/>
     <mergeCell ref="A55:G55"/>
     <mergeCell ref="A57:A65"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A23:G23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3420,7 +3448,7 @@
         <v>88</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3441,16 +3469,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A43088F-BCEF-49C1-995E-3284D137F656}">
-  <dimension ref="A1:D42"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3458,7 +3489,7 @@
         <v>143</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>144</v>
@@ -3467,7 +3498,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39">
         <v>44589</v>
       </c>
@@ -3481,7 +3512,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>44591</v>
       </c>
@@ -3495,7 +3526,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>44591</v>
       </c>
@@ -3517,11 +3548,11 @@
         <v>79</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="D5" s="26"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>44591</v>
       </c>
@@ -3529,56 +3560,106 @@
         <v>79</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="26"/>
+        <v>152</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="A7" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>182</v>
+      </c>
       <c r="D7" s="26"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="A8" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>176</v>
+      </c>
       <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+      <c r="A9" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>177</v>
+      </c>
       <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>179</v>
+      </c>
       <c r="D10" s="26"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>180</v>
+      </c>
       <c r="D11" s="26"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="D12" s="26"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>183</v>
+      </c>
       <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="39">
+        <v>44594</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>184</v>
+      </c>
       <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,7 +3830,18 @@
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
     </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="39"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D13" xr:uid="{4A43088F-BCEF-49C1-995E-3284D137F656}">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3780,7 +3872,7 @@
         <v>144</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3791,10 +3883,10 @@
         <v>79</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>151</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added 1st & 2nd segment checklist to project tracking
</commit_message>
<xml_diff>
--- a/Resources/Project Summary.xlsx
+++ b/Resources/Project Summary.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\msu\20 - Final Project\group_project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0847A0-8B78-4A59-9A0E-C3BBFBC46835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273EC0F8-42DF-4004-B9AF-B537B700B9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12390" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="4" xr2:uid="{241C9D2D-BDEA-4EB4-AA6E-D41C381F1952}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{241C9D2D-BDEA-4EB4-AA6E-D41C381F1952}"/>
   </bookViews>
   <sheets>
     <sheet name="1st Segment" sheetId="14" r:id="rId1"/>
-    <sheet name="Summary" sheetId="8" r:id="rId2"/>
-    <sheet name="Physician Data" sheetId="11" r:id="rId3"/>
-    <sheet name="References" sheetId="9" r:id="rId4"/>
-    <sheet name="Notes" sheetId="12" r:id="rId5"/>
-    <sheet name="Limitations" sheetId="13" r:id="rId6"/>
-    <sheet name="Grade" sheetId="2" r:id="rId7"/>
+    <sheet name="2nd Segment" sheetId="15" r:id="rId2"/>
+    <sheet name="Summary" sheetId="8" r:id="rId3"/>
+    <sheet name="Physician Data" sheetId="11" r:id="rId4"/>
+    <sheet name="References" sheetId="9" r:id="rId5"/>
+    <sheet name="Notes" sheetId="12" r:id="rId6"/>
+    <sheet name="Limitations" sheetId="13" r:id="rId7"/>
+    <sheet name="Grade" sheetId="2" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Notes!$A$1:$D$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Physician Data'!$A$1:$E$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Notes!$A$1:$D$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Physician Data'!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="213">
   <si>
     <t>Project</t>
   </si>
@@ -307,15 +308,9 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Doctors &amp; Clinicians Data</t>
-  </si>
-  <si>
     <t>Topic</t>
   </si>
   <si>
-    <t>Income by Zip Code</t>
-  </si>
-  <si>
     <t>NPI</t>
   </si>
   <si>
@@ -508,9 +503,6 @@
     <t>Resolve issue with pushing to github</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Selected topic </t>
   </si>
   <si>
@@ -536,18 +528,6 @@
   </si>
   <si>
     <t>Machine Learning Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Includes a README.md README.md</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> README.md must include: Description of the communication protocols</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual Branches: At least one branch for each team member </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Each team member has at least four commits from the duration of the first segment</t>
   </si>
   <si>
     <t xml:space="preserve"> Outputs label(s) for input data</t>
@@ -604,6 +584,277 @@
   </si>
   <si>
     <t>How are we handling merges and branches?</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/hamishgunasekara/average-income-per-zip-code-usa-2018</t>
+  </si>
+  <si>
+    <t>https://simplemaps.com/data/us-zips</t>
+  </si>
+  <si>
+    <t>Rev</t>
+  </si>
+  <si>
+    <t>Rev00</t>
+  </si>
+  <si>
+    <t>Rev01</t>
+  </si>
+  <si>
+    <t>Income &amp; Zipcode Data</t>
+  </si>
+  <si>
+    <t>Income &amp; ZCTA Data</t>
+  </si>
+  <si>
+    <t>Physician &amp; Zipcode Data</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Main Branch)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Includes a README.md</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(README.md)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Description of the communication protocols</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Individual Branches)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> At least one branch for each team member </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Individual Branches)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Each team member has at least four commits from the duration of the first segment</t>
+    </r>
+  </si>
+  <si>
+    <t>Presentations are drafted in Google Slides</t>
+  </si>
+  <si>
+    <t>All code in the main branch is production ready</t>
+  </si>
+  <si>
+    <t>Note: The descriptions and explanations required in all other project deliverables 
+should also be in your README.md as part of your outline, unless otherwise noted.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Main Branch)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All code necessary to perform exploratory analysis</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Main Branch)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Some code necessary to complete the machine learning portion of the project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(README.md)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Outline of the project (this may include images, but should be easy to follow and digest)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Individual Branches)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Each team member has at least four commits for the duration 
+of the second segment (eight total commits per person)</t>
+    </r>
+  </si>
+  <si>
+    <t>Description of preliminary data preprocessing</t>
+  </si>
+  <si>
+    <t>Description of preliminary feature engineering and
+preliminary feature selection, including their decision making process</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description of how data was split into training and testing sets</t>
+  </si>
+  <si>
+    <t>A blueprint for the dashboard is created and includes all of the following:</t>
+  </si>
+  <si>
+    <t>Storyboard on Google Slide(s)</t>
+  </si>
+  <si>
+    <t>Description of the tool(s) that will be used to create final dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description of interactive element(s) </t>
+  </si>
+  <si>
+    <t>Team members present a fully integrated database</t>
+  </si>
+  <si>
+    <t>Database stores static data for use during the project</t>
+  </si>
+  <si>
+    <t>Database interfaces with the project in some format (e.g., scraping
+updates the database, or database connects to the model)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes at least two tables (or collections, if using MongoDB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes at least one join using the database language (not including any joins in Pandas) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Includes at least one connection string (using SQLAlchemy or PyMongo)</t>
+  </si>
+  <si>
+    <t>Note: If you use a SQL database, you must provide your ERD with relationships.</t>
+  </si>
+  <si>
+    <t>Machine
+Learning
+Model</t>
   </si>
 </sst>
 </file>
@@ -639,7 +890,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +915,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -1093,7 +1350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1228,7 +1485,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1238,54 +1501,152 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1599,14 +1960,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8BE6C3A-695D-44EF-B92F-86DBEA14E3DC}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1614,183 +1975,622 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C1" s="42" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="49">
+        <v>30</v>
+      </c>
+      <c r="E2" s="46"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="50"/>
+      <c r="B3" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="50"/>
+      <c r="E3" s="47"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
+      <c r="B4" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="50"/>
+      <c r="E4" s="47"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="51"/>
+      <c r="E5" s="48"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="49">
+        <v>10</v>
+      </c>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="47"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="50"/>
+      <c r="B8" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="47"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="47"/>
+    </row>
+    <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="48"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="49">
+        <v>35</v>
+      </c>
+      <c r="E11" s="46"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="47">
-        <v>30</v>
-      </c>
-      <c r="E2" s="50"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="40" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="48"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="51"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="52"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="49">
+        <v>25</v>
+      </c>
+      <c r="E13" s="46"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="44" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="47">
-        <v>10</v>
-      </c>
-      <c r="E6" s="50"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="51"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="51"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="41" t="s">
+      <c r="C14" s="41"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="48"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="52"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="47">
-        <v>35</v>
-      </c>
-      <c r="E10" s="50"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="41" t="s">
+      <c r="B15" s="65" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="52"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="47">
-        <v>25</v>
-      </c>
-      <c r="E12" s="50"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="52"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45">
-        <f>SUM(D2:D13)</f>
+      <c r="C15" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="45">
+        <f>SUM(D2:D14)</f>
         <v>100</v>
       </c>
-      <c r="E14" s="45">
-        <f>SUM(E2:E13)</f>
+      <c r="E15" s="45">
+        <f>SUM(E2:E14)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
   </mergeCells>
+  <conditionalFormatting sqref="C2:C7 C9:C14">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8780AD08-2B49-4EA3-8C7B-9489A8A2B4AB}">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="49">
+        <v>15</v>
+      </c>
+      <c r="E2" s="46"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="50"/>
+      <c r="B3" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="47"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
+      <c r="B4" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="47"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
+      <c r="B5" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="47"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="50"/>
+      <c r="B6" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="47"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="47"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="41"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="48"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="49">
+        <v>10</v>
+      </c>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="66"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="47"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
+      <c r="B11" s="66" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="66"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="47"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
+      <c r="B12" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="66"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="47"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C13" s="66"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="47"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="66"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="47"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="50"/>
+      <c r="B15" s="69" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="66"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="47"/>
+    </row>
+    <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="68" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="48"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" s="44"/>
+      <c r="D17" s="49">
+        <v>30</v>
+      </c>
+      <c r="E17" s="46"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
+      <c r="B18" s="69" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="66"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="47"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="50"/>
+      <c r="B19" s="66" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="66"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="47"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="51"/>
+      <c r="B20" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="48"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" s="44"/>
+      <c r="D21" s="49">
+        <v>30</v>
+      </c>
+      <c r="E21" s="46"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="50"/>
+      <c r="B22" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="66"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="47"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="50"/>
+      <c r="B23" s="69" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" s="66"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="47"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="50"/>
+      <c r="B24" s="67" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="47"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="50"/>
+      <c r="B25" s="67" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="47"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="50"/>
+      <c r="B26" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="47"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="51"/>
+      <c r="B27" s="68" t="s">
+        <v>211</v>
+      </c>
+      <c r="C27" s="41"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="48"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="49">
+        <v>15</v>
+      </c>
+      <c r="E28" s="46"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="50"/>
+      <c r="B29" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="47"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="50"/>
+      <c r="B30" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="47"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="51"/>
+      <c r="B31" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="41"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="48"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="45">
+        <f>SUM(D2:D31)</f>
+        <v>100</v>
+      </c>
+      <c r="E32" s="45">
+        <f>SUM(E2:E31)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="E21:E27"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="D9:D16"/>
+    <mergeCell ref="E9:E16"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:C5 C28 C7:C9 C11 C13:C17 C20 C30:C31">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C19">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:C24 C26:C27">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C852F2-FAA5-4B27-AD13-24C7EB26B87C}">
   <dimension ref="A1:G72"/>
   <sheetViews>
@@ -1807,15 +2607,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -1841,7 +2641,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -1864,7 +2664,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -1885,7 +2685,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
@@ -1896,7 +2696,7 @@
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1917,7 +2717,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
@@ -1928,7 +2728,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
@@ -1939,7 +2739,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
@@ -1950,7 +2750,7 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
@@ -1961,7 +2761,7 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
@@ -1992,7 +2792,7 @@
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="59" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -2005,7 +2805,7 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
@@ -2036,7 +2836,7 @@
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="52" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -2049,7 +2849,7 @@
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
@@ -2060,7 +2860,7 @@
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="57"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
@@ -2091,15 +2891,15 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="55"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -2125,7 +2925,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="52" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -2138,7 +2938,7 @@
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="57"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="9" t="s">
         <v>39</v>
       </c>
@@ -2149,7 +2949,7 @@
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="9" t="s">
         <v>40</v>
       </c>
@@ -2160,7 +2960,7 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="57"/>
+      <c r="A28" s="53"/>
       <c r="B28" s="9" t="s">
         <v>41</v>
       </c>
@@ -2171,7 +2971,7 @@
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="57"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="9" t="s">
         <v>42</v>
       </c>
@@ -2182,7 +2982,7 @@
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="9" t="s">
         <v>43</v>
       </c>
@@ -2202,7 +3002,7 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -2215,7 +3015,7 @@
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="57"/>
+      <c r="A33" s="53"/>
       <c r="B33" s="9" t="s">
         <v>45</v>
       </c>
@@ -2226,7 +3026,7 @@
       <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="9" t="s">
         <v>46</v>
       </c>
@@ -2257,7 +3057,7 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="52" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -2290,15 +3090,15 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="55"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="56"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
@@ -2324,7 +3124,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="59" t="s">
         <v>51</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -2337,7 +3137,7 @@
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="57"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="9" t="s">
         <v>53</v>
       </c>
@@ -2348,7 +3148,7 @@
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="9" t="s">
         <v>54</v>
       </c>
@@ -2359,7 +3159,7 @@
       <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="9" t="s">
         <v>55</v>
       </c>
@@ -2370,7 +3170,7 @@
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="57"/>
+      <c r="A46" s="53"/>
       <c r="B46" s="9" t="s">
         <v>56</v>
       </c>
@@ -2381,7 +3181,7 @@
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
+      <c r="A47" s="53"/>
       <c r="B47" s="9" t="s">
         <v>57</v>
       </c>
@@ -2392,7 +3192,7 @@
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="9" t="s">
         <v>58</v>
       </c>
@@ -2403,7 +3203,7 @@
       <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="9" t="s">
         <v>62</v>
       </c>
@@ -2414,7 +3214,7 @@
       <c r="G49" s="9"/>
     </row>
     <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="57"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="9" t="s">
         <v>63</v>
       </c>
@@ -2425,7 +3225,7 @@
       <c r="G50" s="9"/>
     </row>
     <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="9" t="s">
         <v>61</v>
       </c>
@@ -2436,7 +3236,7 @@
       <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="57"/>
+      <c r="A52" s="53"/>
       <c r="B52" s="9" t="s">
         <v>60</v>
       </c>
@@ -2467,15 +3267,15 @@
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="53" t="s">
+      <c r="A55" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="54"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="55"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="56"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
@@ -2501,7 +3301,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="59" t="s">
         <v>51</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -2514,7 +3314,7 @@
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="57"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="9" t="s">
         <v>71</v>
       </c>
@@ -2525,7 +3325,7 @@
       <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="57"/>
+      <c r="A59" s="53"/>
       <c r="B59" s="9" t="s">
         <v>72</v>
       </c>
@@ -2536,7 +3336,7 @@
       <c r="G59" s="9"/>
     </row>
     <row r="60" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="57"/>
+      <c r="A60" s="53"/>
       <c r="B60" s="9" t="s">
         <v>65</v>
       </c>
@@ -2547,7 +3347,7 @@
       <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="57"/>
+      <c r="A61" s="53"/>
       <c r="B61" s="9" t="s">
         <v>66</v>
       </c>
@@ -2558,7 +3358,7 @@
       <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="57"/>
+      <c r="A62" s="53"/>
       <c r="B62" s="9" t="s">
         <v>67</v>
       </c>
@@ -2569,7 +3369,7 @@
       <c r="G62" s="9"/>
     </row>
     <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="57"/>
+      <c r="A63" s="53"/>
       <c r="B63" s="9" t="s">
         <v>68</v>
       </c>
@@ -2580,7 +3380,7 @@
       <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="57"/>
+      <c r="A64" s="53"/>
       <c r="B64" s="9" t="s">
         <v>69</v>
       </c>
@@ -2611,15 +3411,15 @@
       <c r="G66" s="11"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="53" t="s">
+      <c r="A67" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="54"/>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="55"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="55"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="56"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
@@ -2645,7 +3445,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="56" t="s">
+      <c r="A69" s="59" t="s">
         <v>51</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -2658,7 +3458,7 @@
       <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="57"/>
+      <c r="A70" s="53"/>
       <c r="B70" s="9" t="s">
         <v>76</v>
       </c>
@@ -2669,7 +3469,7 @@
       <c r="G70" s="9"/>
     </row>
     <row r="71" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="57"/>
+      <c r="A71" s="53"/>
       <c r="B71" s="9" t="s">
         <v>77</v>
       </c>
@@ -2692,12 +3492,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A23:G23"/>
     <mergeCell ref="A67:G67"/>
     <mergeCell ref="A69:A72"/>
     <mergeCell ref="A32:A35"/>
@@ -2706,13 +3500,19 @@
     <mergeCell ref="A42:A53"/>
     <mergeCell ref="A55:G55"/>
     <mergeCell ref="A57:A65"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A23:G23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E729EE-DEDD-44FB-892C-76E3520BDE5B}">
   <dimension ref="A1:I41"/>
   <sheetViews>
@@ -2729,24 +3529,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>131</v>
-      </c>
       <c r="D1" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="36">
         <v>0</v>
@@ -2755,7 +3555,7 @@
         <v>83</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>7</v>
@@ -2763,7 +3563,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" s="37">
         <v>0</v>
@@ -2772,7 +3572,7 @@
         <v>83</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>7</v>
@@ -2780,7 +3580,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" s="37">
         <v>0</v>
@@ -2789,7 +3589,7 @@
         <v>83</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>7</v>
@@ -2797,7 +3597,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="37">
         <v>43</v>
@@ -2806,7 +3606,7 @@
         <v>83</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>7</v>
@@ -2814,7 +3614,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="37">
         <v>23</v>
@@ -2823,7 +3623,7 @@
         <v>83</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>7</v>
@@ -2831,7 +3631,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="37">
         <v>666989</v>
@@ -2840,7 +3640,7 @@
         <v>83</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>7</v>
@@ -2848,7 +3648,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="37">
         <v>2343534</v>
@@ -2857,7 +3657,7 @@
         <v>83</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>7</v>
@@ -2865,7 +3665,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="37">
         <v>0</v>
@@ -2874,7 +3674,7 @@
         <v>83</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>7</v>
@@ -2882,7 +3682,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="37">
         <v>1757553</v>
@@ -2891,7 +3691,7 @@
         <v>83</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>7</v>
@@ -2899,7 +3699,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B11" s="37">
         <v>5</v>
@@ -2908,7 +3708,7 @@
         <v>83</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>7</v>
@@ -2916,7 +3716,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="37">
         <v>1448</v>
@@ -2926,12 +3726,12 @@
         <v>7</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B13" s="37">
         <v>0</v>
@@ -2941,12 +3741,12 @@
         <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" s="37">
         <v>2052644</v>
@@ -2955,7 +3755,7 @@
         <v>83</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>7</v>
@@ -2963,7 +3763,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15" s="37">
         <v>2347165</v>
@@ -2972,7 +3772,7 @@
         <v>83</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>7</v>
@@ -2980,7 +3780,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B16" s="37">
         <v>2378739</v>
@@ -2989,7 +3789,7 @@
         <v>83</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>7</v>
@@ -2997,7 +3797,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" s="37">
         <v>2381715</v>
@@ -3006,7 +3806,7 @@
         <v>83</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>7</v>
@@ -3014,7 +3814,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="37">
         <v>2052644</v>
@@ -3023,7 +3823,7 @@
         <v>83</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>7</v>
@@ -3031,7 +3831,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B19" s="37">
         <v>165342</v>
@@ -3040,7 +3840,7 @@
         <v>83</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>7</v>
@@ -3048,7 +3848,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B20" s="37">
         <v>165338</v>
@@ -3057,7 +3857,7 @@
         <v>83</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>7</v>
@@ -3065,7 +3865,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B21" s="37">
         <v>165338</v>
@@ -3074,7 +3874,7 @@
         <v>83</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>7</v>
@@ -3082,7 +3882,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B22" s="37">
         <v>0</v>
@@ -3091,7 +3891,7 @@
         <v>83</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>7</v>
@@ -3099,7 +3899,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B23" s="37">
         <v>1548008</v>
@@ -3108,7 +3908,7 @@
         <v>83</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>7</v>
@@ -3116,7 +3916,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B24" s="37">
         <v>2230224</v>
@@ -3125,7 +3925,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>7</v>
@@ -3133,7 +3933,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B25" s="37">
         <v>0</v>
@@ -3143,12 +3943,12 @@
         <v>7</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B26" s="37">
         <v>0</v>
@@ -3158,12 +3958,12 @@
         <v>7</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B27" s="37">
         <v>0</v>
@@ -3173,12 +3973,12 @@
         <v>7</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B28" s="37">
         <v>369711</v>
@@ -3187,7 +3987,7 @@
         <v>83</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>7</v>
@@ -3196,7 +3996,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B29" s="37">
         <v>716713</v>
@@ -3205,7 +4005,7 @@
         <v>83</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>7</v>
@@ -3214,7 +4014,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B30" s="37">
         <v>759697</v>
@@ -3223,7 +4023,7 @@
         <v>83</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>7</v>
@@ -3231,7 +4031,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B31" s="37">
         <v>1558520</v>
@@ -3240,7 +4040,7 @@
         <v>83</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>7</v>
@@ -3248,7 +4048,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B32" s="37">
         <v>1569520</v>
@@ -3257,7 +4057,7 @@
         <v>83</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>7</v>
@@ -3265,7 +4065,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B33" s="37">
         <v>1953168</v>
@@ -3274,7 +4074,7 @@
         <v>83</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>7</v>
@@ -3282,7 +4082,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B34" s="37">
         <v>1956099</v>
@@ -3291,7 +4091,7 @@
         <v>83</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>7</v>
@@ -3299,7 +4099,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B35" s="37">
         <v>2136049</v>
@@ -3308,7 +4108,7 @@
         <v>83</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>7</v>
@@ -3316,7 +4116,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B36" s="37">
         <v>2137475</v>
@@ -3325,7 +4125,7 @@
         <v>83</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>7</v>
@@ -3333,7 +4133,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B37" s="37">
         <v>2226772</v>
@@ -3342,7 +4142,7 @@
         <v>83</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>7</v>
@@ -3350,7 +4150,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B38" s="37">
         <v>2227317</v>
@@ -3359,7 +4159,7 @@
         <v>83</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>7</v>
@@ -3367,7 +4167,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B39" s="37">
         <v>0</v>
@@ -3377,12 +4177,12 @@
         <v>7</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B40" s="37">
         <v>0</v>
@@ -3392,12 +4192,12 @@
         <v>7</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B41" s="38">
         <v>0</v>
@@ -3406,7 +4206,7 @@
         <v>83</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E41" s="30" t="s">
         <v>7</v>
@@ -3415,7 +4215,7 @@
   </sheetData>
   <autoFilter ref="A1:E41" xr:uid="{F4E729EE-DEDD-44FB-892C-76E3520BDE5B}"/>
   <conditionalFormatting sqref="D2:E41">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3423,57 +4223,99 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06689E2-AD35-403A-B277-1F7A6902B34D}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="78.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>87</v>
+        <v>180</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="C2" s="63">
+        <v>44591</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="63">
+        <v>44592</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="63">
+        <v>44591</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="62"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{A1E8794D-40F3-45CE-BC70-102DA76E9106}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{DA91939A-44E6-4ED6-B36B-FB237141A43B}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{8FE0FD7F-2090-435D-B653-9538C13BA1A2}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{E48266EB-1BB8-4BCE-8B8D-FBFFA76336D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A43088F-BCEF-49C1-995E-3284D137F656}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3486,19 +4328,19 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="39">
         <v>44589</v>
       </c>
@@ -3506,13 +4348,13 @@
         <v>79</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>44591</v>
       </c>
@@ -3520,13 +4362,13 @@
         <v>79</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
         <v>44591</v>
       </c>
@@ -3534,7 +4376,7 @@
         <v>79</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>83</v>
@@ -3548,11 +4390,11 @@
         <v>79</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D5" s="26"/>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
         <v>44591</v>
       </c>
@@ -3560,7 +4402,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>83</v>
@@ -3574,7 +4416,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D7" s="26"/>
     </row>
@@ -3586,7 +4428,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D8" s="26"/>
     </row>
@@ -3598,7 +4440,7 @@
         <v>79</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D9" s="26"/>
     </row>
@@ -3610,9 +4452,11 @@
         <v>79</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="26"/>
+        <v>172</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
@@ -3622,7 +4466,7 @@
         <v>79</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D11" s="26"/>
     </row>
@@ -3634,9 +4478,11 @@
         <v>79</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="D12" s="26"/>
+        <v>174</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
@@ -3646,7 +4492,7 @@
         <v>79</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D13" s="26"/>
     </row>
@@ -3658,7 +4504,7 @@
         <v>79</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D14" s="26"/>
     </row>
@@ -3837,17 +4683,13 @@
       <c r="D43" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D13" xr:uid="{4A43088F-BCEF-49C1-995E-3284D137F656}">
-    <filterColumn colId="3">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D14" xr:uid="{4A43088F-BCEF-49C1-995E-3284D137F656}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEDF1D8-3AEE-4455-9A00-39D4871E0119}">
   <dimension ref="A1:D39"/>
   <sheetViews>
@@ -3863,16 +4705,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>144</v>
-      </c>
       <c r="D1" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3883,10 +4725,10 @@
         <v>79</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4120,7 +4962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6778B80B-57A3-49F9-829D-BD3A1A351548}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -4150,7 +4992,7 @@
         <v>0.19</v>
       </c>
       <c r="C2" s="6">
-        <f>'1st Segment'!E14</f>
+        <f>'1st Segment'!E15</f>
         <v>0</v>
       </c>
     </row>
@@ -4161,7 +5003,10 @@
       <c r="B3" s="5">
         <v>0.19</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6">
+        <f>'2nd Segment'!E32</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
rev 05 and physician data input
</commit_message>
<xml_diff>
--- a/Resources/Project Summary.xlsx
+++ b/Resources/Project Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony\msu\20 - Final Project\group_project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273EC0F8-42DF-4004-B9AF-B537B700B9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B637818-F107-49C6-A00B-53D5EC90D183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{241C9D2D-BDEA-4EB4-AA6E-D41C381F1952}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="214">
   <si>
     <t>Project</t>
   </si>
@@ -855,6 +855,9 @@
     <t>Machine
 Learning
 Model</t>
+  </si>
+  <si>
+    <t>Identifier for physicians</t>
   </si>
 </sst>
 </file>
@@ -1431,13 +1434,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1485,6 +1482,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1502,6 +1532,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1529,50 +1562,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -1980,178 +1976,178 @@
       <c r="B1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="41" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="49">
+      <c r="C2" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="58">
         <v>30</v>
       </c>
-      <c r="E2" s="46"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="40" t="s">
+      <c r="A3" s="59"/>
+      <c r="B3" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="59"/>
+      <c r="E3" s="56"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="47"/>
+      <c r="C4" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="59"/>
+      <c r="E4" s="56"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="41" t="s">
+      <c r="A5" s="60"/>
+      <c r="B5" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="48"/>
+      <c r="C5" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="60"/>
+      <c r="E5" s="57"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="49">
+      <c r="C6" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="58">
         <v>10</v>
       </c>
-      <c r="E6" s="46"/>
+      <c r="E6" s="55"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="59"/>
+      <c r="B7" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="47"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="56"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="40" t="s">
+      <c r="A8" s="59"/>
+      <c r="B8" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="47"/>
+      <c r="C8" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="59"/>
+      <c r="E8" s="56"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="40" t="s">
+      <c r="A9" s="59"/>
+      <c r="B9" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="C9" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="47"/>
+      <c r="C9" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="59"/>
+      <c r="E9" s="56"/>
     </row>
     <row r="10" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="68" t="s">
+      <c r="A10" s="60"/>
+      <c r="B10" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="48"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="57"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="49">
+      <c r="C11" s="42"/>
+      <c r="D11" s="58">
         <v>35</v>
       </c>
-      <c r="E11" s="46"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="41" t="s">
+      <c r="A12" s="60"/>
+      <c r="B12" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="48"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="57"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="49">
+      <c r="C13" s="42"/>
+      <c r="D13" s="58">
         <v>25</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="55"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="41" t="s">
+      <c r="A14" s="60"/>
+      <c r="B14" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="48"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="57"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D15" s="43">
         <f>SUM(D2:D14)</f>
         <v>100</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="43">
         <f>SUM(E2:E14)</f>
         <v>0</v>
       </c>
@@ -2172,12 +2168,12 @@
     <mergeCell ref="D13:D14"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C7 C9:C14">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2208,332 +2204,327 @@
       <c r="B1" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="41" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="49">
+      <c r="C2" s="42"/>
+      <c r="D2" s="58">
         <v>15</v>
       </c>
-      <c r="E2" s="46"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="66" t="s">
+      <c r="A3" s="59"/>
+      <c r="B3" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="56"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="66" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="47"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="56"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="59"/>
+      <c r="B5" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="47"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="56"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="67" t="s">
+      <c r="A6" s="59"/>
+      <c r="B6" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="47"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="56"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="67" t="s">
+      <c r="A7" s="59"/>
+      <c r="B7" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="47"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="56"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="41" t="s">
+      <c r="A8" s="60"/>
+      <c r="B8" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="48"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="57"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="49">
+      <c r="C9" s="42"/>
+      <c r="D9" s="58">
         <v>10</v>
       </c>
-      <c r="E9" s="46"/>
+      <c r="E9" s="55"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="66" t="s">
+      <c r="A10" s="59"/>
+      <c r="B10" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="47"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="56"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="66" t="s">
+      <c r="A11" s="59"/>
+      <c r="B11" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="47"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="56"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="40" t="s">
+      <c r="A12" s="59"/>
+      <c r="B12" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="47"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="56"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="40" t="s">
+      <c r="A13" s="59"/>
+      <c r="B13" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="47"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="56"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="40" t="s">
+      <c r="A14" s="59"/>
+      <c r="B14" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="47"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="56"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="69" t="s">
+      <c r="A15" s="59"/>
+      <c r="B15" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="47"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="56"/>
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="68" t="s">
+      <c r="A16" s="60"/>
+      <c r="B16" s="51" t="s">
         <v>193</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="48"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="57"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="49">
+      <c r="C17" s="42"/>
+      <c r="D17" s="58">
         <v>30</v>
       </c>
-      <c r="E17" s="46"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="69" t="s">
+      <c r="A18" s="59"/>
+      <c r="B18" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="47"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="56"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="66" t="s">
+      <c r="A19" s="59"/>
+      <c r="B19" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="47"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="56"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="41" t="s">
+      <c r="A20" s="60"/>
+      <c r="B20" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="48"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="57"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="49">
+      <c r="C21" s="42"/>
+      <c r="D21" s="58">
         <v>30</v>
       </c>
-      <c r="E21" s="46"/>
+      <c r="E21" s="55"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="69" t="s">
+      <c r="A22" s="59"/>
+      <c r="B22" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="C22" s="66"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="47"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="56"/>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="69" t="s">
+      <c r="A23" s="59"/>
+      <c r="B23" s="52" t="s">
         <v>207</v>
       </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="47"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="56"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="67" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="47"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="56"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="67" t="s">
+      <c r="A25" s="59"/>
+      <c r="B25" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="47"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="56"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="67" t="s">
+      <c r="A26" s="59"/>
+      <c r="B26" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="47"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="56"/>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="68" t="s">
+      <c r="A27" s="60"/>
+      <c r="B27" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="48"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="57"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="49">
+      <c r="C28" s="42"/>
+      <c r="D28" s="58">
         <v>15</v>
       </c>
-      <c r="E28" s="46"/>
+      <c r="E28" s="55"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="40" t="s">
+      <c r="A29" s="59"/>
+      <c r="B29" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="47"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="56"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="40" t="s">
+      <c r="A30" s="59"/>
+      <c r="B30" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="47"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="56"/>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="41" t="s">
+      <c r="A31" s="60"/>
+      <c r="B31" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="48"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="57"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="B32" s="65" t="s">
+      <c r="B32" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="48" t="s">
         <v>167</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="43">
         <f>SUM(D2:D31)</f>
         <v>100</v>
       </c>
-      <c r="E32" s="45">
+      <c r="E32" s="43">
         <f>SUM(E2:E31)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="D21:D27"/>
-    <mergeCell ref="E21:E27"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="D17:D20"/>
     <mergeCell ref="E17:E20"/>
@@ -2544,9 +2535,14 @@
     <mergeCell ref="A9:A16"/>
     <mergeCell ref="D9:D16"/>
     <mergeCell ref="E9:E16"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="D21:D27"/>
+    <mergeCell ref="E21:E27"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C5 C28 C7:C9 C11 C13:C17 C20 C30:C31">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2581,7 +2577,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2607,15 +2603,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="56"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -2641,7 +2637,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="67" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -2664,7 +2660,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
@@ -2685,7 +2681,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
@@ -2696,7 +2692,7 @@
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
@@ -2717,7 +2713,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
@@ -2728,7 +2724,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
@@ -2739,7 +2735,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
@@ -2750,7 +2746,7 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
@@ -2761,7 +2757,7 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
@@ -2772,7 +2768,7 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58"/>
+      <c r="A12" s="68"/>
       <c r="B12" s="10" t="s">
         <v>19</v>
       </c>
@@ -2792,7 +2788,7 @@
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="69" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -2805,7 +2801,7 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
@@ -2816,7 +2812,7 @@
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="58"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="10" t="s">
         <v>23</v>
       </c>
@@ -2836,7 +2832,7 @@
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="62" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -2849,7 +2845,7 @@
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="63"/>
       <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
@@ -2860,7 +2856,7 @@
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
@@ -2871,7 +2867,7 @@
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
+      <c r="A21" s="68"/>
       <c r="B21" s="10" t="s">
         <v>28</v>
       </c>
@@ -2891,15 +2887,15 @@
       <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="56"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="66"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
@@ -2925,7 +2921,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="62" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -2938,7 +2934,7 @@
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="9" t="s">
         <v>39</v>
       </c>
@@ -2949,7 +2945,7 @@
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="9" t="s">
         <v>40</v>
       </c>
@@ -2960,7 +2956,7 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53"/>
+      <c r="A28" s="63"/>
       <c r="B28" s="9" t="s">
         <v>41</v>
       </c>
@@ -2971,7 +2967,7 @@
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="9" t="s">
         <v>42</v>
       </c>
@@ -2982,7 +2978,7 @@
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="A30" s="63"/>
       <c r="B30" s="9" t="s">
         <v>43</v>
       </c>
@@ -3002,7 +2998,7 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="69" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="8" t="s">
@@ -3015,7 +3011,7 @@
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
+      <c r="A33" s="63"/>
       <c r="B33" s="9" t="s">
         <v>45</v>
       </c>
@@ -3026,7 +3022,7 @@
       <c r="G33" s="9"/>
     </row>
     <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="60"/>
+      <c r="A34" s="70"/>
       <c r="B34" s="9" t="s">
         <v>46</v>
       </c>
@@ -3037,7 +3033,7 @@
       <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="58"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="10" t="s">
         <v>47</v>
       </c>
@@ -3057,7 +3053,7 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="52" t="s">
+      <c r="A37" s="62" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -3070,7 +3066,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="58"/>
+      <c r="A38" s="68"/>
       <c r="B38" s="10" t="s">
         <v>49</v>
       </c>
@@ -3090,15 +3086,15 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="55"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="56"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="66"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
@@ -3124,7 +3120,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="59" t="s">
+      <c r="A42" s="69" t="s">
         <v>51</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -3137,7 +3133,7 @@
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="53"/>
+      <c r="A43" s="63"/>
       <c r="B43" s="9" t="s">
         <v>53</v>
       </c>
@@ -3148,7 +3144,7 @@
       <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="53"/>
+      <c r="A44" s="63"/>
       <c r="B44" s="9" t="s">
         <v>54</v>
       </c>
@@ -3159,7 +3155,7 @@
       <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="9" t="s">
         <v>55</v>
       </c>
@@ -3170,7 +3166,7 @@
       <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="53"/>
+      <c r="A46" s="63"/>
       <c r="B46" s="9" t="s">
         <v>56</v>
       </c>
@@ -3181,7 +3177,7 @@
       <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="53"/>
+      <c r="A47" s="63"/>
       <c r="B47" s="9" t="s">
         <v>57</v>
       </c>
@@ -3192,7 +3188,7 @@
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="53"/>
+      <c r="A48" s="63"/>
       <c r="B48" s="9" t="s">
         <v>58</v>
       </c>
@@ -3203,7 +3199,7 @@
       <c r="G48" s="9"/>
     </row>
     <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53"/>
+      <c r="A49" s="63"/>
       <c r="B49" s="9" t="s">
         <v>62</v>
       </c>
@@ -3214,7 +3210,7 @@
       <c r="G49" s="9"/>
     </row>
     <row r="50" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="53"/>
+      <c r="A50" s="63"/>
       <c r="B50" s="9" t="s">
         <v>63</v>
       </c>
@@ -3225,7 +3221,7 @@
       <c r="G50" s="9"/>
     </row>
     <row r="51" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="53"/>
+      <c r="A51" s="63"/>
       <c r="B51" s="9" t="s">
         <v>61</v>
       </c>
@@ -3236,7 +3232,7 @@
       <c r="G51" s="9"/>
     </row>
     <row r="52" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="53"/>
+      <c r="A52" s="63"/>
       <c r="B52" s="9" t="s">
         <v>60</v>
       </c>
@@ -3247,7 +3243,7 @@
       <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="58"/>
+      <c r="A53" s="68"/>
       <c r="B53" s="10" t="s">
         <v>59</v>
       </c>
@@ -3267,15 +3263,15 @@
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="54" t="s">
+      <c r="A55" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="56"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="66"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
@@ -3301,7 +3297,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="59" t="s">
+      <c r="A57" s="69" t="s">
         <v>51</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -3314,7 +3310,7 @@
       <c r="G57" s="8"/>
     </row>
     <row r="58" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="53"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="9" t="s">
         <v>71</v>
       </c>
@@ -3325,7 +3321,7 @@
       <c r="G58" s="9"/>
     </row>
     <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="53"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="9" t="s">
         <v>72</v>
       </c>
@@ -3336,7 +3332,7 @@
       <c r="G59" s="9"/>
     </row>
     <row r="60" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="53"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="9" t="s">
         <v>65</v>
       </c>
@@ -3347,7 +3343,7 @@
       <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="53"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="9" t="s">
         <v>66</v>
       </c>
@@ -3358,7 +3354,7 @@
       <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="53"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="9" t="s">
         <v>67</v>
       </c>
@@ -3369,7 +3365,7 @@
       <c r="G62" s="9"/>
     </row>
     <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="53"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="9" t="s">
         <v>68</v>
       </c>
@@ -3380,7 +3376,7 @@
       <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="53"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="9" t="s">
         <v>69</v>
       </c>
@@ -3391,7 +3387,7 @@
       <c r="G64" s="9"/>
     </row>
     <row r="65" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="58"/>
+      <c r="A65" s="68"/>
       <c r="B65" s="10" t="s">
         <v>73</v>
       </c>
@@ -3411,15 +3407,15 @@
       <c r="G66" s="11"/>
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="55"/>
-      <c r="D67" s="55"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="55"/>
-      <c r="G67" s="56"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="65"/>
+      <c r="D67" s="65"/>
+      <c r="E67" s="65"/>
+      <c r="F67" s="65"/>
+      <c r="G67" s="66"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
@@ -3445,7 +3441,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="59" t="s">
+      <c r="A69" s="69" t="s">
         <v>51</v>
       </c>
       <c r="B69" s="8" t="s">
@@ -3458,7 +3454,7 @@
       <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="53"/>
+      <c r="A70" s="63"/>
       <c r="B70" s="9" t="s">
         <v>76</v>
       </c>
@@ -3469,7 +3465,7 @@
       <c r="G70" s="9"/>
     </row>
     <row r="71" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="53"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="9" t="s">
         <v>77</v>
       </c>
@@ -3480,7 +3476,7 @@
       <c r="G71" s="9"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="58"/>
+      <c r="A72" s="68"/>
       <c r="B72" s="10" t="s">
         <v>78</v>
       </c>
@@ -3514,9 +3510,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E729EE-DEDD-44FB-892C-76E3520BDE5B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3531,41 +3530,39 @@
       <c r="A1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="33" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="34">
         <v>0</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="33" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="37">
+      <c r="B3" s="35">
         <v>0</v>
       </c>
       <c r="C3" s="26" t="s">
@@ -3578,11 +3575,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B4" s="35">
         <v>0</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -3595,11 +3592,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="35">
         <v>43</v>
       </c>
       <c r="C5" s="26" t="s">
@@ -3612,11 +3609,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="35">
         <v>23</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -3629,11 +3626,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="35">
         <v>666989</v>
       </c>
       <c r="C7" s="26" t="s">
@@ -3646,11 +3643,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="35">
         <v>2343534</v>
       </c>
       <c r="C8" s="26" t="s">
@@ -3663,11 +3660,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="35">
         <v>0</v>
       </c>
       <c r="C9" s="26" t="s">
@@ -3680,11 +3677,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="35">
         <v>1757553</v>
       </c>
       <c r="C10" s="26" t="s">
@@ -3697,11 +3694,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="37">
+      <c r="B11" s="35">
         <v>5</v>
       </c>
       <c r="C11" s="26" t="s">
@@ -3718,7 +3715,7 @@
       <c r="A12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="35">
         <v>1448</v>
       </c>
       <c r="C12" s="26"/>
@@ -3733,7 +3730,7 @@
       <c r="A13" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="37">
+      <c r="B13" s="35">
         <v>0</v>
       </c>
       <c r="C13" s="26"/>
@@ -3744,11 +3741,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="37">
+      <c r="B14" s="35">
         <v>2052644</v>
       </c>
       <c r="C14" s="26" t="s">
@@ -3761,11 +3758,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="35">
         <v>2347165</v>
       </c>
       <c r="C15" s="26" t="s">
@@ -3778,11 +3775,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="37">
+      <c r="B16" s="35">
         <v>2378739</v>
       </c>
       <c r="C16" s="26" t="s">
@@ -3795,11 +3792,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="37">
+      <c r="B17" s="35">
         <v>2381715</v>
       </c>
       <c r="C17" s="26" t="s">
@@ -3812,11 +3809,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="37">
+      <c r="B18" s="35">
         <v>2052644</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -3829,11 +3826,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="37">
+      <c r="B19" s="35">
         <v>165342</v>
       </c>
       <c r="C19" s="26" t="s">
@@ -3846,11 +3843,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B20" s="35">
         <v>165338</v>
       </c>
       <c r="C20" s="26" t="s">
@@ -3863,11 +3860,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="37">
+      <c r="B21" s="35">
         <v>165338</v>
       </c>
       <c r="C21" s="26" t="s">
@@ -3880,11 +3877,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="37">
+      <c r="B22" s="35">
         <v>0</v>
       </c>
       <c r="C22" s="26" t="s">
@@ -3897,11 +3894,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="37">
+      <c r="B23" s="35">
         <v>1548008</v>
       </c>
       <c r="C23" s="26" t="s">
@@ -3914,11 +3911,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="37">
+      <c r="B24" s="35">
         <v>2230224</v>
       </c>
       <c r="C24" s="26" t="s">
@@ -3935,7 +3932,7 @@
       <c r="A25" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="37">
+      <c r="B25" s="35">
         <v>0</v>
       </c>
       <c r="C25" s="26"/>
@@ -3950,7 +3947,7 @@
       <c r="A26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="37">
+      <c r="B26" s="35">
         <v>0</v>
       </c>
       <c r="C26" s="26"/>
@@ -3965,7 +3962,7 @@
       <c r="A27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B27" s="35">
         <v>0</v>
       </c>
       <c r="C27" s="26"/>
@@ -3976,11 +3973,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="37">
+      <c r="B28" s="35">
         <v>369711</v>
       </c>
       <c r="C28" s="26" t="s">
@@ -3994,11 +3991,11 @@
       </c>
       <c r="I28" s="27"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B29" s="35">
         <v>716713</v>
       </c>
       <c r="C29" s="26" t="s">
@@ -4012,11 +4009,11 @@
       </c>
       <c r="I29" s="27"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="37">
+      <c r="B30" s="35">
         <v>759697</v>
       </c>
       <c r="C30" s="26" t="s">
@@ -4029,11 +4026,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="37">
+      <c r="B31" s="35">
         <v>1558520</v>
       </c>
       <c r="C31" s="26" t="s">
@@ -4046,11 +4043,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="37">
+      <c r="B32" s="35">
         <v>1569520</v>
       </c>
       <c r="C32" s="26" t="s">
@@ -4063,11 +4060,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="37">
+      <c r="B33" s="35">
         <v>1953168</v>
       </c>
       <c r="C33" s="26" t="s">
@@ -4080,11 +4077,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="37">
+      <c r="B34" s="35">
         <v>1956099</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -4097,11 +4094,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="37">
+      <c r="B35" s="35">
         <v>2136049</v>
       </c>
       <c r="C35" s="26" t="s">
@@ -4114,11 +4111,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="37">
+      <c r="B36" s="35">
         <v>2137475</v>
       </c>
       <c r="C36" s="26" t="s">
@@ -4131,11 +4128,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B37" s="37">
+      <c r="B37" s="35">
         <v>2226772</v>
       </c>
       <c r="C37" s="26" t="s">
@@ -4148,11 +4145,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="37">
+      <c r="B38" s="35">
         <v>2227317</v>
       </c>
       <c r="C38" s="26" t="s">
@@ -4169,7 +4166,7 @@
       <c r="A39" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="37">
+      <c r="B39" s="35">
         <v>0</v>
       </c>
       <c r="C39" s="26"/>
@@ -4184,7 +4181,7 @@
       <c r="A40" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B40" s="37">
+      <c r="B40" s="35">
         <v>0</v>
       </c>
       <c r="C40" s="26"/>
@@ -4195,31 +4192,36 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
+    <row r="41" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="38">
+      <c r="B41" s="36">
         <v>0</v>
       </c>
-      <c r="C41" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" s="29" t="s">
+      <c r="C41" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="54" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E41" xr:uid="{F4E729EE-DEDD-44FB-892C-76E3520BDE5B}"/>
+  <autoFilter ref="A1:E41" xr:uid="{F4E729EE-DEDD-44FB-892C-76E3520BDE5B}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="D2:E41">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4258,7 +4260,7 @@
       <c r="B2" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C2" s="63">
+      <c r="C2" s="46">
         <v>44591</v>
       </c>
       <c r="D2" s="25" t="s">
@@ -4272,7 +4274,7 @@
       <c r="B3" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="63">
+      <c r="C3" s="46">
         <v>44592</v>
       </c>
       <c r="D3" s="25" t="s">
@@ -4286,7 +4288,7 @@
       <c r="B4" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="46">
         <v>44591</v>
       </c>
       <c r="D4" s="25" t="s">
@@ -4294,10 +4296,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="62"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="45"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4341,7 +4343,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="39">
+      <c r="A2" s="37">
         <v>44589</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -4355,7 +4357,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
+      <c r="A3" s="37">
         <v>44591</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -4369,7 +4371,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="39">
+      <c r="A4" s="37">
         <v>44591</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -4383,7 +4385,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="39">
+      <c r="A5" s="37">
         <v>44591</v>
       </c>
       <c r="B5" s="26" t="s">
@@ -4395,7 +4397,7 @@
       <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="37">
         <v>44591</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -4409,7 +4411,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="37">
         <v>44594</v>
       </c>
       <c r="B7" s="26" t="s">
@@ -4421,7 +4423,7 @@
       <c r="D7" s="26"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
+      <c r="A8" s="37">
         <v>44594</v>
       </c>
       <c r="B8" s="26" t="s">
@@ -4433,7 +4435,7 @@
       <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+      <c r="A9" s="37">
         <v>44594</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -4445,7 +4447,7 @@
       <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
+      <c r="A10" s="37">
         <v>44594</v>
       </c>
       <c r="B10" s="26" t="s">
@@ -4459,7 +4461,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="37">
         <v>44594</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -4471,7 +4473,7 @@
       <c r="D11" s="26"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="37">
         <v>44594</v>
       </c>
       <c r="B12" s="26" t="s">
@@ -4485,7 +4487,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="39">
+      <c r="A13" s="37">
         <v>44594</v>
       </c>
       <c r="B13" s="26" t="s">
@@ -4497,7 +4499,7 @@
       <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="A14" s="37">
         <v>44594</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -4509,175 +4511,175 @@
       <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="39"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="39"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="39"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="39"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="39"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="39"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
       <c r="D41" s="26"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
+      <c r="A43" s="37"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
       <c r="D43" s="26"/>
@@ -4718,7 +4720,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="39">
+      <c r="A2" s="37">
         <v>44591</v>
       </c>
       <c r="B2" s="26" t="s">
@@ -4732,223 +4734,223 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
       <c r="D7" s="26"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
       <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
       <c r="D11" s="26"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
       <c r="D17" s="26"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="39"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
       <c r="D30" s="26"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="39"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="26"/>
       <c r="C33" s="26"/>
       <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="39"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="26"/>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="26"/>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="39"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="26"/>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="26"/>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="39"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="26"/>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>

</xml_diff>